<commit_message>
Automatische test-sync: 2025-08-01 22:59:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-01.xlsx
+++ b/logs/mail_log_2025-08-01.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -738,8 +738,63 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank je wel voor je e-mail. Kun je alsjeblieft meer details geven over wat je precies geregeld wilt hebben? Op die manier kan ik je beter helpen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-08-01 22:59:31</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -759,7 +814,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -767,17 +822,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -819,7 +874,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:01:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-01.xlsx
+++ b/logs/mail_log_2025-08-01.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -793,8 +793,64 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, zou u wat meer specifieke informatie kunnen verstrekken over wat u precies geregeld wilt hebben?
+Met vriendelijke groet,
+[Jouw naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-08-01 23:01:32</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -814,7 +870,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -822,17 +878,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -874,7 +930,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:36:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-01.xlsx
+++ b/logs/mail_log_2025-08-01.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -905,8 +905,60 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-08-01 23:36:06</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -926,7 +978,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -934,17 +986,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -986,7 +1038,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:38:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-01.xlsx
+++ b/logs/mail_log_2025-08-01.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -957,8 +957,63 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Beste,
+Dank voor je bericht. Kun je wat meer context geven over wat je precies bedoelt met "Testmail #2" en wat er van mij verwacht wordt om op te pakken? Graag hoor ik meer details, zodat ik je beter van dienst kan zijn.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-08-01 23:38:18</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -978,7 +1033,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -986,17 +1041,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J6">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1011,7 +1066,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1041,6 +1096,16 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:41:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-01.xlsx
+++ b/logs/mail_log_2025-08-01.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1012,8 +1012,60 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Testmail #3: Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-08-01 23:40:52</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1033,7 +1085,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1041,17 +1093,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="J2:J8">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1093,7 +1145,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:45:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-01.xlsx
+++ b/logs/mail_log_2025-08-01.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1116,8 +1116,64 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Wil je deze klant bellen?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Testmail #5: Wil je deze klant bellen?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Beste,
+Bedankt voor uw bericht. Om u beter van dienst te kunnen zijn, zou ik graag wat meer informatie willen ontvangen. Kunt u mij alstublieft de naam van de klant en het telefoonnummer doorgeven, zodat wij contact met hen kunnen opnemen?
+Met vriendelijke groet,
+[Jouw Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-08-01 23:45:13</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1137,7 +1193,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1145,17 +1201,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
+  <conditionalFormatting sqref="J2:J10">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1207,7 +1263,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:47:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-01.xlsx
+++ b/logs/mail_log_2025-08-01.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1172,8 +1172,63 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Hebben we EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Testmail #6: Hebben we EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Hartelijk dank voor uw e-mail. Op dit moment hebben we nog EcoPro-700 op voorraad. U kunt deze bestellen via onze website of neem contact met ons op voor verdere assistentie.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-08-01 23:47:25</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1193,7 +1248,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1201,17 +1256,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J10">
+  <conditionalFormatting sqref="J2:J11">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1226,7 +1281,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1276,6 +1331,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:49:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-01.xlsx
+++ b/logs/mail_log_2025-08-01.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1227,8 +1227,60 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Testmail #7: Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-08-01 23:49:37</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1248,7 +1300,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1256,17 +1308,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1324,17 +1376,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:52:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-01.xlsx
+++ b/logs/mail_log_2025-08-01.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1279,8 +1279,64 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Kun je nagaan of dit nog leverbaar is?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Testmail #8: Kun je nagaan of dit nog leverbaar is?</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Om uw vraag over de leverbaarheid te beantwoorden, hebben we meer informatie nodig over het specifieke product waar u naar informeert. Kunt u ons de naam of het artikelnummer van het product geven?
+Zodra we deze informatie hebben, zullen we direct voor u nakijken of het product nog leverbaar is. Alvast bedankt voor uw medewerking.
+Met vriendelijke groet,
+[Bedrijfsnaam] e-mailassistent</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-08-01 23:51:50</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1300,7 +1356,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1308,17 +1364,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I13">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J12">
+  <conditionalFormatting sqref="J2:J13">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1366,17 +1422,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Intern verzoek / Actie voor medewerker</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:54:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-01.xlsx
+++ b/logs/mail_log_2025-08-01.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1335,8 +1335,60 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Testmail #9: Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-08-01 23:54:01</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1356,7 +1408,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1364,17 +1416,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H13">
+  <conditionalFormatting sqref="H2:H14">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I13">
+  <conditionalFormatting sqref="I2:I14">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J13">
+  <conditionalFormatting sqref="J2:J14">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1416,7 +1468,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:56:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-01.xlsx
+++ b/logs/mail_log_2025-08-01.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1387,8 +1387,60 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Testmail #10: Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-08-01 23:56:11</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1408,7 +1460,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1416,17 +1468,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:H15">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
+  <conditionalFormatting sqref="I2:I15">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J14">
+  <conditionalFormatting sqref="J2:J15">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1468,7 +1520,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-01 23:58:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-01.xlsx
+++ b/logs/mail_log_2025-08-01.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1439,8 +1439,68 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Mijn retour is nog steeds niet verwerkt.</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Testmail #11: Mijn retour is nog steeds niet verwerkt.</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Ik begrijp uw zorgen over de verwerking van uw retourzending. Om u beter van dienst te kunnen zijn, heb ik wat meer informatie nodig. Kunt u alstublieft het volgende verstrekken:
+1. Het ordernummer van uw aankoop.
+2. De datum waarop u de retour heeft verzonden.
+3. Eventuele traceerinformatie van de retourzending.
+Met deze gegevens kunnen we verder onderzoek doen naar de status van uw retour en u zo snel mogelijk een update geven.
+Ik kijk uit naar uw reactie.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-08-01 23:58:23</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1460,7 +1520,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1468,17 +1528,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H15">
+  <conditionalFormatting sqref="H2:H16">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I15">
+  <conditionalFormatting sqref="I2:I16">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J15">
+  <conditionalFormatting sqref="J2:J16">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1493,7 +1553,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1553,6 +1613,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>